<commit_message>
Different Hourly rates on different projects implemented
</commit_message>
<xml_diff>
--- a/Portefølje_F2026.xlsx
+++ b/Portefølje_F2026.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Portefølje_F2026" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Timesatser_budget" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -731,7 +732,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="C8" t="n">
         <v>437</v>
@@ -740,10 +741,10 @@
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>221</v>
       </c>
       <c r="F8" t="n">
-        <v>121</v>
+        <v>0</v>
       </c>
       <c r="G8" t="n">
         <v>658</v>
@@ -766,11 +767,11 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>NN</t>
+          <t>NN (ufordelt)</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>277</v>
+        <v>375</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
@@ -779,17 +780,23 @@
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>211</v>
+        <v>267</v>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
+        <v>93</v>
       </c>
       <c r="G9" t="n">
-        <v>488</v>
-      </c>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
+        <v>735</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>9265</v>
+      </c>
+      <c r="J9" t="n">
+        <v>10000</v>
+      </c>
       <c r="K9" t="inlineStr">
         <is>
           <t>F2026</t>
@@ -799,7 +806,7 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>*** Sum projektløn [kr]</t>
+          <t>*** Projektbudget [kr]</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -827,6 +834,286 @@
         </is>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>*** Sum projektløn [kr]</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>369670</v>
+      </c>
+      <c r="C11" t="n">
+        <v>230940</v>
+      </c>
+      <c r="D11" t="n">
+        <v>398530</v>
+      </c>
+      <c r="E11" t="n">
+        <v>299881</v>
+      </c>
+      <c r="F11" t="n">
+        <v>149954</v>
+      </c>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>F2026</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Medarbejder</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>The Change</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>LEG-DHC</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>LTDE-repBC</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>COOLGEOHEAT II</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>HEATCODE</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Søren Erbs Poulsen (SOEB)</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>638.89</v>
+      </c>
+      <c r="C2" t="n">
+        <v>638.89</v>
+      </c>
+      <c r="D2" t="n">
+        <v>656.64</v>
+      </c>
+      <c r="E2" t="n">
+        <v>414.98</v>
+      </c>
+      <c r="F2" t="n">
+        <v>716.77</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Mathias Larsen (MATL)</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>531.36</v>
+      </c>
+      <c r="C3" t="n">
+        <v>531.36</v>
+      </c>
+      <c r="D3" t="n">
+        <v>531.3099999999999</v>
+      </c>
+      <c r="E3" t="n">
+        <v>342.31</v>
+      </c>
+      <c r="F3" t="n">
+        <v>596.1322093005057</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Rune Kier Nielsen (RUNI)</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>582.9400000000001</v>
+      </c>
+      <c r="C4" t="n">
+        <v>582.9400000000001</v>
+      </c>
+      <c r="D4" t="n">
+        <v>582.9400000000001</v>
+      </c>
+      <c r="E4" t="n">
+        <v>343.67</v>
+      </c>
+      <c r="F4" t="n">
+        <v>653.9997555134688</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Kristoffer Bested Nielsen (KRI)</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>472.53</v>
+      </c>
+      <c r="C5" t="n">
+        <v>472.53</v>
+      </c>
+      <c r="D5" t="n">
+        <v>499.35</v>
+      </c>
+      <c r="E5" t="n">
+        <v>303.95</v>
+      </c>
+      <c r="F5" t="n">
+        <v>529.5599999999999</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Søren Andersen (SSSA)</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>531.36</v>
+      </c>
+      <c r="C6" t="n">
+        <v>531.36</v>
+      </c>
+      <c r="D6" t="n">
+        <v>531.36</v>
+      </c>
+      <c r="E6" t="n">
+        <v>342.31</v>
+      </c>
+      <c r="F6" t="n">
+        <v>596.1322093005057</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Karl Woldum Tordrup (KART)</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>584.08</v>
+      </c>
+      <c r="C7" t="n">
+        <v>584.08</v>
+      </c>
+      <c r="D7" t="n">
+        <v>584.08</v>
+      </c>
+      <c r="E7" t="n">
+        <v>383.05</v>
+      </c>
+      <c r="F7" t="n">
+        <v>655.27</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Marton Major (MMAJ)</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>531.36</v>
+      </c>
+      <c r="C8" t="n">
+        <v>529.01</v>
+      </c>
+      <c r="D8" t="n">
+        <v>529.01</v>
+      </c>
+      <c r="E8" t="n">
+        <v>345.1357397987135</v>
+      </c>
+      <c r="F8" t="n">
+        <v>596.1322093005057</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>NN (ufordelt)</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>535.9</v>
+      </c>
+      <c r="C9" t="n">
+        <v>535.9</v>
+      </c>
+      <c r="D9" t="n">
+        <v>570.24</v>
+      </c>
+      <c r="E9" t="n">
+        <v>404.93</v>
+      </c>
+      <c r="F9" t="n">
+        <v>601.225630390208</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Project budget [DKR]</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>369670</v>
+      </c>
+      <c r="C10" t="n">
+        <v>230940</v>
+      </c>
+      <c r="D10" t="n">
+        <v>398530</v>
+      </c>
+      <c r="E10" t="n">
+        <v>299881</v>
+      </c>
+      <c r="F10" t="n">
+        <v>149954</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Now supports preallocation of fixed amount of hours
</commit_message>
<xml_diff>
--- a/Portefølje_F2026.xlsx
+++ b/Portefølje_F2026.xlsx
@@ -498,25 +498,25 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="D2" t="n">
-        <v>607</v>
+        <v>508</v>
       </c>
       <c r="E2" t="n">
-        <v>51</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>657</v>
+        <v>608</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
@@ -546,16 +546,16 @@
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>208</v>
+        <v>658</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>208</v>
+        <v>658</v>
       </c>
       <c r="H3" t="n">
-        <v>450</v>
+        <v>0</v>
       </c>
       <c r="I3" t="n">
         <v>0</v>
@@ -582,10 +582,10 @@
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>112</v>
       </c>
       <c r="E4" t="n">
-        <v>178</v>
+        <v>66</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
@@ -594,13 +594,13 @@
         <v>178</v>
       </c>
       <c r="H4" t="n">
-        <v>0</v>
+        <v>480</v>
       </c>
       <c r="I4" t="n">
         <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>178</v>
+        <v>658</v>
       </c>
       <c r="K4" t="inlineStr">
         <is>
@@ -732,16 +732,16 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0</v>
+        <v>227</v>
       </c>
       <c r="C8" t="n">
-        <v>437</v>
+        <v>376</v>
       </c>
       <c r="D8" t="n">
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>221</v>
+        <v>54</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
@@ -771,7 +771,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>581</v>
+        <v>296</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
@@ -780,20 +780,18 @@
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>91</v>
+        <v>0</v>
       </c>
       <c r="F9" t="n">
         <v>93</v>
       </c>
       <c r="G9" t="n">
-        <v>765</v>
+        <v>389</v>
       </c>
       <c r="H9" t="n">
         <v>0</v>
       </c>
-      <c r="I9" t="n">
-        <v>9235</v>
-      </c>
+      <c r="I9" t="inlineStr"/>
       <c r="J9" t="n">
         <v>10000</v>
       </c>
@@ -841,16 +839,16 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>369766</v>
+        <v>369598</v>
       </c>
       <c r="C11" t="n">
-        <v>231177</v>
+        <v>230852</v>
       </c>
       <c r="D11" t="n">
-        <v>398580</v>
+        <v>398862</v>
       </c>
       <c r="E11" t="n">
-        <v>300096</v>
+        <v>299994</v>
       </c>
       <c r="F11" t="n">
         <v>150103</v>

</xml_diff>

<commit_message>
Further minor improvements and labelling
</commit_message>
<xml_diff>
--- a/Portefølje_F2026.xlsx
+++ b/Portefølje_F2026.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Portefølje_F2026" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Timesatser_budget" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Timesatser" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -498,25 +498,25 @@
         </is>
       </c>
       <c r="B2" t="n">
+        <v>200</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>408</v>
+      </c>
+      <c r="E2" t="n">
         <v>50</v>
       </c>
-      <c r="C2" t="n">
-        <v>50</v>
-      </c>
-      <c r="D2" t="n">
-        <v>508</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
       <c r="F2" t="n">
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>608</v>
+        <v>658</v>
       </c>
       <c r="H2" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
@@ -582,10 +582,10 @@
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>112</v>
+        <v>178</v>
       </c>
       <c r="E4" t="n">
-        <v>66</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
@@ -732,16 +732,16 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>227</v>
+        <v>110</v>
       </c>
       <c r="C8" t="n">
-        <v>376</v>
+        <v>437</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="E8" t="n">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
@@ -771,7 +771,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>296</v>
+        <v>234</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
@@ -786,7 +786,7 @@
         <v>93</v>
       </c>
       <c r="G9" t="n">
-        <v>389</v>
+        <v>327</v>
       </c>
       <c r="H9" t="n">
         <v>0</v>
@@ -804,7 +804,7 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>*** Projektbudget [kr]</t>
+          <t>Projektbudget [kr]</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -835,20 +835,20 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>*** Sum projektløn [kr]</t>
+          <t>Projektomkostning [kr]</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>369598</v>
+        <v>370036</v>
       </c>
       <c r="C11" t="n">
-        <v>230852</v>
+        <v>231177</v>
       </c>
       <c r="D11" t="n">
-        <v>398862</v>
+        <v>399181</v>
       </c>
       <c r="E11" t="n">
-        <v>299994</v>
+        <v>299786</v>
       </c>
       <c r="F11" t="n">
         <v>150103</v>

</xml_diff>